<commit_message>
selenium homework - personal details
</commit_message>
<xml_diff>
--- a/Files/PersonalDetails.xlsx
+++ b/Files/PersonalDetails.xlsx
@@ -253,19 +253,19 @@
     <t>DL02468135</t>
   </si>
   <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>024-68-1357</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>1995</t>
+  </si>
+  <si>
     <t>Jan</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>024-68-1357</t>
-  </si>
-  <si>
-    <t>German</t>
-  </si>
-  <si>
-    <t>1995</t>
   </si>
   <si>
     <t>Sophia</t>
@@ -293,7 +293,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -301,6 +308,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -314,6 +328,66 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -322,8 +396,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -331,14 +413,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -346,59 +421,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -411,29 +434,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -444,13 +444,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -462,169 +624,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,11 +640,18 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -664,6 +671,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -673,20 +695,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -706,32 +725,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -740,7 +740,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -758,130 +758,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1241,7 +1241,7 @@
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5"/>
@@ -1600,13 +1600,13 @@
         <v>25</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="J6" t="s">
         <v>80</v>
-      </c>
-      <c r="J6" t="s">
-        <v>81</v>
       </c>
       <c r="K6">
         <v>123456789</v>
@@ -1618,13 +1618,13 @@
         <v>30</v>
       </c>
       <c r="N6" t="s">
+        <v>81</v>
+      </c>
+      <c r="O6" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="P6" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="Q6" s="10" t="s">
         <v>33</v>

</xml_diff>